<commit_message>
Popravke scenarija, i razdvajanje foldera za scenarije i dijagrame.
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Login Vlasnika.xlsx
+++ b/UseCaseScenarij/Login Vlasnika.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alem\KlixNightlife\UseCaseScenarij\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Naziv</t>
   </si>
@@ -59,36 +54,12 @@
     <t>Administrator</t>
   </si>
   <si>
-    <t>Login vlasnika</t>
-  </si>
-  <si>
-    <t>Mora biti registrovan kao vlasnik.</t>
-  </si>
-  <si>
-    <t>Korisnik se prijavljuje; Dodaje objekat</t>
-  </si>
-  <si>
-    <t>Korisnikov  nije unio tacne podatke za prijavu; Administrator odbija dodavanje objekta</t>
-  </si>
-  <si>
-    <t>Zavrsava uspješno kada se vlasnik prijavi ili doda svoj objekat.</t>
-  </si>
-  <si>
     <t>1. Pristupa interfejsu za prijavu</t>
   </si>
   <si>
-    <t>2. Upisuje username i sifru</t>
-  </si>
-  <si>
     <t>3. Provjerava ispravnost podataka za prijavu</t>
   </si>
   <si>
-    <t>Vlasnik zeli da doda svoj objekat ili da gleda sadrzaj kao logovan korisnik.</t>
-  </si>
-  <si>
-    <t>4. Postaje logovani korisnik</t>
-  </si>
-  <si>
     <t>Tok dogadjaja - Login uspješan</t>
   </si>
   <si>
@@ -98,25 +69,37 @@
     <t>Preduvjet: Vlasnik zeli da doda svoj objekat</t>
   </si>
   <si>
-    <t>1. Popunjava podatke o objektu</t>
-  </si>
-  <si>
-    <t>2. Salje zahtjev za dodavanje objekta</t>
-  </si>
-  <si>
-    <t>4. Salje zahtjev administratoru</t>
-  </si>
-  <si>
-    <t>5. Provjerava podatke o objektu</t>
-  </si>
-  <si>
-    <t>6. Odobrava ili ne odobrava dodavanje objekta</t>
-  </si>
-  <si>
-    <t>7. Salje povratnu informaciju vlasniku</t>
-  </si>
-  <si>
-    <t>8. Nastavlja na stavku broj 4. standardnog toka događaja.</t>
+    <t>Nema</t>
+  </si>
+  <si>
+    <t>Vlasnik objekta zeli da se registuje.</t>
+  </si>
+  <si>
+    <t>Vlasnik je registrovan, i moze izvrsiti login</t>
+  </si>
+  <si>
+    <t>Vlasnik dobija mail o razlogu odbijanja</t>
+  </si>
+  <si>
+    <t>Zavrsava uspjesno kada administrator odobri registraciju vlasnika</t>
+  </si>
+  <si>
+    <t>Registracija vlasnika</t>
+  </si>
+  <si>
+    <t>2. Upisuje licne podatke</t>
+  </si>
+  <si>
+    <t>4. Odobrava registraciju vlasnika</t>
+  </si>
+  <si>
+    <t>5. Registruje se, sada može login</t>
+  </si>
+  <si>
+    <t>4. Neodobrava registraciju vlasnika</t>
+  </si>
+  <si>
+    <t>5. Šalje mu mail sa razlogom</t>
   </si>
 </sst>
 </file>
@@ -206,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -234,9 +217,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -257,15 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -327,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,7 +521,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,11 +532,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -573,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -581,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -589,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -597,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,12 +585,12 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -637,14 +608,14 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -652,45 +623,47 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="14"/>
+      <c r="A18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
@@ -704,23 +677,23 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>25</v>
+      <c r="A21" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="4"/>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -728,94 +701,90 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="2"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="11"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="11"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="11"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="11"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="11"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="11"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="11"/>
+      <c r="C39" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+Scenarij registrovanja novog korisnika
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Login Vlasnika.xlsx
+++ b/UseCaseScenarij/Login Vlasnika.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Naziv</t>
   </si>
@@ -63,12 +63,6 @@
     <t>Tok dogadjaja - Login uspješan</t>
   </si>
   <si>
-    <t>Alternativni tok dogadjaja - Dodavanje objekta</t>
-  </si>
-  <si>
-    <t>Preduvjet: Vlasnik zeli da doda svoj objekat</t>
-  </si>
-  <si>
     <t>Nema</t>
   </si>
   <si>
@@ -99,7 +93,10 @@
     <t>4. Neodobrava registraciju vlasnika</t>
   </si>
   <si>
-    <t>5. Šalje mu mail sa razlogom</t>
+    <t>Alternativni tok dogadjaja - Login neuspješan</t>
+  </si>
+  <si>
+    <t>5. Šalje se mail vlasniku sa razlogom</t>
   </si>
 </sst>
 </file>
@@ -133,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -162,26 +159,166 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -189,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,46 +334,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,7 +688,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,259 +699,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>21</v>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>22</v>
+      <c r="A11" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
+      <c r="C13" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="20"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="13"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>22</v>
+      <c r="A21" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="14"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="10"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="10"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>